<commit_message>
- (WIP) Done with (very) rough draft of basic setup analysis in report - Removed getBigramCount method - Replaced sentence 28 with a more accurate translation
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realn\OneDrive\Documents\git\comp472_mp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906A19F1-1D03-4AEC-8F78-CDF9624DE7E3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4234C6-D8B2-4CA6-8D0A-039488A0340F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6880" xr2:uid="{B453E516-9AC6-4D84-BB36-529AE5470C70}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6880" activeTab="5" xr2:uid="{B453E516-9AC6-4D84-BB36-529AE5470C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic" sheetId="1" r:id="rId1"/>
-    <sheet name="Ex4" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId2"/>
+    <sheet name="Ex1" sheetId="4" r:id="rId3"/>
+    <sheet name="Ex2" sheetId="5" r:id="rId4"/>
+    <sheet name="Ex3" sheetId="7" r:id="rId5"/>
+    <sheet name="Ex4" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="87">
   <si>
     <t>Birds build nests.</t>
   </si>
@@ -167,6 +171,132 @@
   </si>
   <si>
     <t>T'es sur de ca?</t>
+  </si>
+  <si>
+    <t>Fablo mio Cid bien e tan mesurado: / &lt;&lt;grado a ti, Senor Padre, que estas en alto!&gt;&gt; / Esto me an buelto mios enemigos malos.&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carles li reis, nostre emper[er]e magnes / Set anz tuz pleins ad estet en Espaigne: / Tresqu'en la mer cunquist la tere altaigne. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oft Scyld Scefing sceathena threatum / monegum maegthum meodosetla ofteah, egsode eorl, sythan aerest weard / feasceaft funden. </t>
+  </si>
+  <si>
+    <t>Dime cuenta d'ello al cuartu dia cuandu me dixisti pela mananina: _Comu me presten les atapecies!</t>
+  </si>
+  <si>
+    <t>S'lon le recensement d'2001 y'avait 2,674 personnes tchi palent l'Jerriais (3.2% d'la population).</t>
+  </si>
+  <si>
+    <t>Le jouo va s' dejuqui, le cyil est d'exces rouoge.</t>
+  </si>
+  <si>
+    <t>J'i apprins chu morce de ta vie le quatriyime jouo, des petra-jaquet, quaund tu m'as announchi : J'aime byin les couchis de sole !</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We wad like tae mak shair that as mony fowk as possible can get tae speir aboot the Scots Pairlament. </t>
+  </si>
+  <si>
+    <t>I amna fou' sae muckle as tired - deid dune.</t>
+  </si>
+  <si>
+    <t>I lairnt this new detail on the mornin o the fowert day, whan ye said tae me: I'm awfy fond o doungangs.</t>
+  </si>
+  <si>
+    <t>L'oxetu del alcuerdu ye la promocion, l'espardimientu y la normalizacion llinguistica de la llingua asturiana na institucion academica.</t>
+  </si>
+  <si>
+    <t>Santa Olaya fo l'abeya / que de Merida ensamo.</t>
+  </si>
+  <si>
+    <t>Ki sa ki pral vini ekonomi an Japone ane ca?</t>
+  </si>
+  <si>
+    <t>Li te mande l si li te yon elev nan lekol sa.</t>
+  </si>
+  <si>
+    <t>Mwen OK.</t>
+  </si>
+  <si>
+    <t>Zwazo bati nich.</t>
+  </si>
+  <si>
+    <t>Zwazo vole.</t>
+  </si>
+  <si>
+    <t>Mwen rayi AI.</t>
+  </si>
+  <si>
+    <t>Woody Allen pale.</t>
+  </si>
+  <si>
+    <t>eske abite la?</t>
+  </si>
+  <si>
+    <t>Fraz sa a se nan angle.</t>
+  </si>
+  <si>
+    <t>Mwen renmen AI.</t>
+  </si>
+  <si>
+    <t>AYITI: NOUVO GOUVENMAN AN AP KONFWONTE DEFI SOU KESYON DWA MOUN</t>
+  </si>
+  <si>
+    <t>Se pou limye fet. Epi limye te fet.</t>
+  </si>
+  <si>
+    <t>M aprann sa nan maten katriyem jou a, le w di m : Mwen renmen we soley kouche.</t>
+  </si>
+  <si>
+    <t>Predicted class log probability (U)</t>
+  </si>
+  <si>
+    <t>Predicted class log probability (B)</t>
+  </si>
+  <si>
+    <t>Actual class log probability (U)</t>
+  </si>
+  <si>
+    <t>Actual class log probability (B)</t>
+  </si>
+  <si>
+    <t>Predicted class approximation (U)</t>
+  </si>
+  <si>
+    <t>Actual class approximation (U)</t>
+  </si>
+  <si>
+    <t>Predicted class approximation (B)</t>
+  </si>
+  <si>
+    <t>Actual class approximation (B)</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The weather in Taumata[…] is lovely. </t>
+  </si>
+  <si>
+    <t>Ve a buscar el kayac.</t>
+  </si>
+  <si>
+    <t>Voy a buscar el kayak.</t>
   </si>
 </sst>
 </file>
@@ -246,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -256,6 +386,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CAECAB-4BA0-488D-8A1F-6586C507048E}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -588,9 +721,13 @@
     <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="17.08984375" customWidth="1"/>
+    <col min="9" max="9" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -606,8 +743,20 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -624,7 +773,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -641,7 +790,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -658,7 +807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -674,8 +823,14 @@
       <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>-19.670653611610199</v>
+      </c>
+      <c r="G5">
+        <v>-19.810415665181299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -692,7 +847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -708,8 +863,14 @@
       <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>-13.293184626199499</v>
+      </c>
+      <c r="G7">
+        <v>-13.4776794985341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -725,8 +886,20 @@
       <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>-19.663675869227401</v>
+      </c>
+      <c r="G8">
+        <v>-22.445584235353898</v>
+      </c>
+      <c r="H8">
+        <v>-17.363519046143502</v>
+      </c>
+      <c r="I8">
+        <v>-19.6833787030987</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -743,7 +916,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -759,8 +932,14 @@
       <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <v>-27.138588783522302</v>
+      </c>
+      <c r="G10">
+        <v>-27.301452238145199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -776,8 +955,14 @@
       <c r="E11" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <v>-10.720744118556601</v>
+      </c>
+      <c r="G11">
+        <v>-10.7294752973899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -794,7 +979,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -811,7 +996,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -828,7 +1013,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -845,7 +1030,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1071,13 +1256,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>21</v>
@@ -1149,11 +1334,776 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA19E8C2-4F04-4E47-B4CD-A839DA925246}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="A9:B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="18.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>-19.670653611610199</v>
+      </c>
+      <c r="C2">
+        <v>-19.810415665181299</v>
+      </c>
+      <c r="D2">
+        <v>-17.976177186744199</v>
+      </c>
+      <c r="E2">
+        <v>-17.976177186744199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>-13.293184626199499</v>
+      </c>
+      <c r="C3">
+        <v>-13.4776794985341</v>
+      </c>
+      <c r="D3">
+        <v>-11.1051683500498</v>
+      </c>
+      <c r="E3">
+        <v>-11.1051683500498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>-19.663675869227401</v>
+      </c>
+      <c r="C4">
+        <v>-22.445584235353898</v>
+      </c>
+      <c r="D4">
+        <v>-17.363519046143502</v>
+      </c>
+      <c r="E4">
+        <v>-19.6833787030987</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>-27.138588783522302</v>
+      </c>
+      <c r="C5">
+        <v>-27.301452238145199</v>
+      </c>
+      <c r="D5">
+        <v>-24.2615176871372</v>
+      </c>
+      <c r="E5">
+        <v>-24.2615176871372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>-10.720744118556601</v>
+      </c>
+      <c r="C6">
+        <v>-10.7294752973899</v>
+      </c>
+      <c r="D6">
+        <v>-8.2017680497423502</v>
+      </c>
+      <c r="E6">
+        <v>-8.2017680497423502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42315EAA-DA0E-42CF-9AA1-3C10326EBBED}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE88203F-1989-497E-87B6-3D7004CF1E80}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F15ED4D-BD51-470B-9DC7-962207276B2F}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.453125" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71224B5-21D4-4D35-A8F1-AA4A367A358A}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1646,13 +2596,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>17</v>
+        <v>86</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>20</v>
+      <c r="D29" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Report draft 1 sorta done
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\realn\OneDrive\Documents\git\comp472_mp3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4234C6-D8B2-4CA6-8D0A-039488A0340F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28AB125-146E-4D21-B0F6-A51B5BA75F33}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6880" activeTab="5" xr2:uid="{B453E516-9AC6-4D84-BB36-529AE5470C70}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="93">
   <si>
     <t>Birds build nests.</t>
   </si>
@@ -89,9 +89,6 @@
     <t>El internet de las cosas.</t>
   </si>
   <si>
-    <t>Conseguir el kayac.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Numismatic symmetry should not antagonize economic acme. </t>
   </si>
   <si>
@@ -290,13 +287,34 @@
     <t>S6</t>
   </si>
   <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
     <t xml:space="preserve">The weather in Taumata[…] is lovely. </t>
   </si>
   <si>
-    <t>Ve a buscar el kayac.</t>
-  </si>
-  <si>
     <t>Voy a buscar el kayak.</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>P(k)</t>
+  </si>
+  <si>
+    <t>P(w)</t>
+  </si>
+  <si>
+    <t>P(h|w)</t>
+  </si>
+  <si>
+    <t>Oft Scyld Scefing sceathena threatum / monegum maegthum meodosetla ofteah, egsode eorl, sythan aerest weard / feasceaft funden</t>
   </si>
 </sst>
 </file>
@@ -376,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -388,6 +406,28 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,25 +775,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>72</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -761,16 +801,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -778,16 +818,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -795,16 +835,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -815,13 +855,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <v>-19.670653611610199</v>
@@ -835,16 +875,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -855,13 +895,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7">
         <v>-13.293184626199499</v>
@@ -878,13 +918,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>-19.663675869227401</v>
@@ -904,16 +944,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -924,13 +964,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10">
         <v>-27.138588783522302</v>
@@ -947,13 +987,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11">
         <v>-10.720744118556601</v>
@@ -967,16 +1007,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -984,16 +1024,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1001,16 +1041,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1018,16 +1058,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1035,16 +1075,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1052,16 +1092,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1069,16 +1109,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1086,16 +1126,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1103,16 +1143,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1123,13 +1163,13 @@
         <v>9</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1140,13 +1180,13 @@
         <v>10</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1157,13 +1197,13 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1174,13 +1214,13 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1191,13 +1231,13 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1208,13 +1248,13 @@
         <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1225,13 +1265,13 @@
         <v>15</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1242,13 +1282,13 @@
         <v>16</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1256,16 +1296,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1273,16 +1313,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1293,38 +1333,38 @@
         <v>6</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1335,16 +1375,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA19E8C2-4F04-4E47-B4CD-A839DA925246}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:AD37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="A9:B15"/>
+    <sheetView topLeftCell="U27" workbookViewId="0">
+      <selection activeCell="AB28" sqref="AB28:AD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="18.1796875" customWidth="1"/>
+    <col min="8" max="8" width="61.90625" customWidth="1"/>
+    <col min="28" max="28" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="61.54296875" customWidth="1"/>
+    <col min="30" max="30" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1352,16 +1396,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1459,15 +1503,15 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>5</v>
@@ -1475,34 +1519,232 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="11">
+        <v>2.9067377170496298E-4</v>
+      </c>
+      <c r="C19">
+        <v>4.58514433431378E-3</v>
+      </c>
+      <c r="D19">
+        <v>1.5625E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>8.45868488671115E-3</v>
+      </c>
+      <c r="C20">
+        <v>2.33693161114376E-2</v>
+      </c>
+      <c r="D20">
+        <v>0.26718017414601403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11">
+        <v>6.2422440118153196E-7</v>
+      </c>
+      <c r="C21" s="11">
+        <v>2.1410896960526499E-4</v>
+      </c>
+      <c r="D21">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="G23" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="G24" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="G25" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="G26" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AB28" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD28" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="AB29" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC29" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD29" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="AB30" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC30" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD30" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="AB31" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC31" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD31" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="AB32" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC32" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD32" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="28:30" x14ac:dyDescent="0.35">
+      <c r="AB33" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC33" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD33" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="28:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="AB34" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC34" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD34" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="28:30" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AB35" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>17</v>
+      <c r="AC35" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD35" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="28:30" x14ac:dyDescent="0.35">
+      <c r="AB36" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC36" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD36" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="28:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="AB37" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC37" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD37" s="15" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1516,7 +1758,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B9"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1536,10 +1778,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1550,16 +1792,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1567,16 +1809,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1584,31 +1826,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1621,7 +1863,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1641,10 +1883,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1655,16 +1897,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1672,16 +1914,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1689,16 +1931,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1706,16 +1948,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1723,16 +1965,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1740,16 +1982,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1757,16 +1999,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1774,16 +2016,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1791,31 +2033,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1828,7 +2070,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1848,10 +2090,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1862,16 +2104,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1879,16 +2121,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1896,16 +2138,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1913,16 +2155,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1930,16 +2172,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1947,16 +2189,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1964,16 +2206,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1981,16 +2223,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -1998,16 +2240,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -2015,16 +2257,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -2032,16 +2274,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -2049,16 +2291,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -2066,31 +2308,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2100,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71224B5-21D4-4D35-A8F1-AA4A367A358A}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2113,9 +2355,11 @@
     <col min="3" max="3" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2123,67 +2367,107 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="H1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2191,33 +2475,53 @@
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2225,16 +2529,26 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2242,33 +2556,53 @@
         <v>5</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2276,16 +2610,16 @@
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2293,169 +2627,193 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2463,16 +2821,16 @@
         <v>9</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2480,16 +2838,16 @@
         <v>10</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2497,16 +2855,16 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2514,16 +2872,16 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2531,16 +2889,16 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2548,16 +2906,16 @@
         <v>14</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2565,16 +2923,16 @@
         <v>15</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2582,50 +2940,50 @@
         <v>16</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2633,43 +2991,43 @@
         <v>6</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>